<commit_message>
lot of trial and error
</commit_message>
<xml_diff>
--- a/sgRNA-insert pairs design/Example_Data/alaA_mutations.xlsx
+++ b/sgRNA-insert pairs design/Example_Data/alaA_mutations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unitc-my.sharepoint.com/personal/kxmts01_cloud_uni-tuebingen_de/Documents/Dokumente/GitHub/CREATE_WebApplicaltion/sgRNA-insert pairs design/Example_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="11_6A69D6BF87905768E7B93411598328B1640BEF3A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{692A7D81-0472-424A-9BBE-74DA556DCD80}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="11_6A69D6BF87905768E7B93411598328B1640BEF3A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DEAC7817-E669-4741-B159-73609FF296D3}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -633,8 +633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -966,13 +966,13 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C24" t="s">
         <v>19</v>
       </c>
       <c r="D24">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -980,13 +980,13 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C25" t="s">
         <v>19</v>
       </c>
       <c r="D25">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1022,13 +1022,13 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="C28" t="s">
         <v>11</v>
       </c>
       <c r="D28">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1036,13 +1036,13 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="C29" t="s">
         <v>11</v>
       </c>
       <c r="D29">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>